<commit_message>
Update sample file of result.py and add mpl.py
</commit_message>
<xml_diff>
--- a/result.xlsx
+++ b/result.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21425"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A79A169-88A9-4D48-9EB5-EC146235E96F}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{821F70FE-E16A-4A5F-A37F-1AD4DEC2A130}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="252" yWindow="192" windowWidth="12936" windowHeight="11964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="6">
   <si>
     <t>Suspiciousness</t>
   </si>
@@ -32,6 +32,12 @@
   </si>
   <si>
     <t>Frequency</t>
+  </si>
+  <si>
+    <t>Errortype</t>
+  </si>
+  <si>
+    <t>LOC</t>
   </si>
 </sst>
 </file>
@@ -349,15 +355,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D38"/>
+  <dimension ref="A1:F38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -370,8 +376,14 @@
       <c r="D1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>13</v>
       </c>
@@ -384,8 +396,14 @@
       <c r="D2">
         <v>4500</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E2">
+        <v>1</v>
+      </c>
+      <c r="F2">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>9</v>
       </c>
@@ -393,7 +411,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>15</v>
       </c>
@@ -401,7 +419,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>14</v>
       </c>
@@ -409,7 +427,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>12</v>
       </c>
@@ -417,7 +435,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>11</v>
       </c>
@@ -425,7 +443,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>10</v>
       </c>
@@ -433,7 +451,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>8</v>
       </c>
@@ -441,7 +459,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>7</v>
       </c>
@@ -449,7 +467,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>6</v>
       </c>
@@ -457,7 +475,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>5</v>
       </c>
@@ -465,7 +483,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>4</v>
       </c>
@@ -473,7 +491,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>3</v>
       </c>
@@ -481,7 +499,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>2</v>
       </c>
@@ -489,7 +507,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>18</v>
       </c>

</xml_diff>